<commit_message>
promo overlay msrp tests added
</commit_message>
<xml_diff>
--- a/Data Files/stagingMSRPs.xlsx
+++ b/Data Files/stagingMSRPs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zsmith/Desktop/katalon git repo/datasheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zsmith/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420E8E87-10B3-3541-B1FF-DEC8ECE22939}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F7B3681-B9D5-F849-B316-90A8E8C3F1C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="100">
   <si>
     <t>RC 300 RWD</t>
   </si>
@@ -276,12 +276,6 @@
     <t>LC HYBRID</t>
   </si>
   <si>
-    <t>9260 (SE)</t>
-  </si>
-  <si>
-    <t>LC Inspiration Series</t>
-  </si>
-  <si>
     <t>UX 200 FWD</t>
   </si>
   <si>
@@ -322,6 +316,15 @@
   </si>
   <si>
     <t>GS F</t>
+  </si>
+  <si>
+    <t>LC Convertible</t>
+  </si>
+  <si>
+    <t>9262SE</t>
+  </si>
+  <si>
+    <t>LC Convertible Inspiration Series</t>
   </si>
 </sst>
 </file>
@@ -650,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73:D78"/>
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -665,19 +668,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" t="s">
         <v>93</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>94</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>95</v>
-      </c>
-      <c r="D1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1223,7 +1226,7 @@
         <v>2020</v>
       </c>
       <c r="D34" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E34" s="1">
         <v>1295</v>
@@ -1237,7 +1240,7 @@
         <v>43</v>
       </c>
       <c r="C35">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D35" s="2">
         <v>36870</v>
@@ -1254,7 +1257,7 @@
         <v>44</v>
       </c>
       <c r="C36">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D36" s="2">
         <v>38270</v>
@@ -1271,7 +1274,7 @@
         <v>45</v>
       </c>
       <c r="C37">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D37" s="2">
         <v>39110</v>
@@ -1288,7 +1291,7 @@
         <v>46</v>
       </c>
       <c r="C38">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D38" s="2">
         <v>40510</v>
@@ -1305,7 +1308,7 @@
         <v>47</v>
       </c>
       <c r="C39">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D39" s="2">
         <v>43960</v>
@@ -1322,7 +1325,7 @@
         <v>48</v>
       </c>
       <c r="C40">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D40" s="2">
         <v>45360</v>
@@ -1339,7 +1342,7 @@
         <v>49</v>
       </c>
       <c r="C41">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D41" s="2">
         <v>39420</v>
@@ -1356,7 +1359,7 @@
         <v>50</v>
       </c>
       <c r="C42">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D42" s="2">
         <v>46510</v>
@@ -1373,10 +1376,10 @@
         <v>52</v>
       </c>
       <c r="C43">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D43" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E43" s="1">
         <v>1025</v>
@@ -1390,7 +1393,7 @@
         <v>54</v>
       </c>
       <c r="C44">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D44" s="2">
         <v>46110</v>
@@ -1733,7 +1736,7 @@
         <v>2020</v>
       </c>
       <c r="D64" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E64" s="1">
         <v>1025</v>
@@ -1750,7 +1753,7 @@
         <v>2020</v>
       </c>
       <c r="D65" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E65" s="1">
         <v>1025</v>
@@ -1832,7 +1835,7 @@
         <v>81</v>
       </c>
       <c r="C70">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D70" s="2">
         <v>92950</v>
@@ -1849,7 +1852,7 @@
         <v>82</v>
       </c>
       <c r="C71">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D71" s="2">
         <v>97510</v>
@@ -1859,17 +1862,17 @@
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>83</v>
+      <c r="A72">
+        <v>9262</v>
       </c>
       <c r="B72" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="C72">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D72" s="2">
-        <v>103080</v>
+        <v>101000</v>
       </c>
       <c r="E72" s="1">
         <v>1025</v>
@@ -1880,7 +1883,7 @@
         <v>9720</v>
       </c>
       <c r="B73" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C73">
         <v>2020</v>
@@ -1897,7 +1900,7 @@
         <v>9724</v>
       </c>
       <c r="B74" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C74">
         <v>2020</v>
@@ -1914,7 +1917,7 @@
         <v>9732</v>
       </c>
       <c r="B75" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C75">
         <v>2020</v>
@@ -1931,7 +1934,7 @@
         <v>9736</v>
       </c>
       <c r="B76" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C76">
         <v>2020</v>
@@ -1948,7 +1951,7 @@
         <v>9722</v>
       </c>
       <c r="B77" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C77">
         <v>2020</v>
@@ -1965,7 +1968,7 @@
         <v>9738</v>
       </c>
       <c r="B78" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C78">
         <v>2020</v>
@@ -1982,7 +1985,7 @@
         <v>9335</v>
       </c>
       <c r="B79" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C79">
         <v>2020</v>
@@ -1991,6 +1994,23 @@
         <v>85010</v>
       </c>
       <c r="E79" s="1">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>98</v>
+      </c>
+      <c r="B80" t="s">
+        <v>99</v>
+      </c>
+      <c r="C80">
+        <v>2021</v>
+      </c>
+      <c r="D80" s="2">
+        <v>119800</v>
+      </c>
+      <c r="E80" s="1">
         <v>1025</v>
       </c>
     </row>

</xml_diff>

<commit_message>
nx compare re-enabled; updated gx/lx msrp values added
</commit_message>
<xml_diff>
--- a/Data Files/stagingMSRPs.xlsx
+++ b/Data Files/stagingMSRPs.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zsmith/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmith\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1206DDCD-DA0E-D146-9F1D-CBF7C100383D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="13200"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="98">
   <si>
     <t>RC 300 RWD</t>
   </si>
@@ -324,7 +323,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
@@ -649,21 +648,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
     <col min="4" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>88</v>
       </c>
@@ -680,7 +679,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>9202</v>
       </c>
@@ -697,7 +696,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>9203</v>
       </c>
@@ -714,7 +713,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>9206</v>
       </c>
@@ -731,7 +730,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9207</v>
       </c>
@@ -748,7 +747,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>9212</v>
       </c>
@@ -765,7 +764,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>9213</v>
       </c>
@@ -782,7 +781,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9216</v>
       </c>
@@ -799,7 +798,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9217</v>
       </c>
@@ -816,7 +815,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9000</v>
       </c>
@@ -833,7 +832,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9002</v>
       </c>
@@ -850,7 +849,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9004</v>
       </c>
@@ -867,7 +866,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9040</v>
       </c>
@@ -884,7 +883,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>9042</v>
       </c>
@@ -901,7 +900,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>9044</v>
       </c>
@@ -918,7 +917,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>9005</v>
       </c>
@@ -935,7 +934,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>9502</v>
       </c>
@@ -952,7 +951,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -969,7 +968,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>9506</v>
       </c>
@@ -986,7 +985,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1003,7 +1002,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>9510</v>
       </c>
@@ -1020,7 +1019,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1037,7 +1036,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>9516</v>
       </c>
@@ -1054,7 +1053,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1071,7 +1070,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -1085,7 +1084,7 @@
         <v>45200</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1099,7 +1098,7 @@
         <v>47250</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1113,7 +1112,7 @@
         <v>49415</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1127,7 +1126,7 @@
         <v>50155</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>9700</v>
       </c>
@@ -1138,13 +1137,13 @@
         <v>2020</v>
       </c>
       <c r="D29" s="2">
-        <v>53000</v>
+        <v>53100</v>
       </c>
       <c r="E29" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -1155,13 +1154,13 @@
         <v>2020</v>
       </c>
       <c r="D30" s="2">
-        <v>55790</v>
+        <v>55890</v>
       </c>
       <c r="E30" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>9710</v>
       </c>
@@ -1172,13 +1171,13 @@
         <v>2020</v>
       </c>
       <c r="D31" s="2">
-        <v>64265</v>
+        <v>64365</v>
       </c>
       <c r="E31" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>9625</v>
       </c>
@@ -1189,13 +1188,13 @@
         <v>2020</v>
       </c>
       <c r="D32" s="2">
-        <v>86480</v>
+        <v>86580</v>
       </c>
       <c r="E32" s="1">
-        <v>1295</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>9620</v>
       </c>
@@ -1206,13 +1205,13 @@
         <v>2020</v>
       </c>
       <c r="D33" s="2">
-        <v>91480</v>
+        <v>91580</v>
       </c>
       <c r="E33" s="1">
-        <v>1295</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -1222,14 +1221,14 @@
       <c r="C34">
         <v>2020</v>
       </c>
-      <c r="D34" t="s">
-        <v>87</v>
+      <c r="D34" s="2">
+        <v>94475</v>
       </c>
       <c r="E34" s="1">
-        <v>1295</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>9820</v>
       </c>
@@ -1246,7 +1245,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>9824</v>
       </c>
@@ -1263,7 +1262,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>9830</v>
       </c>
@@ -1280,7 +1279,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>9834</v>
       </c>
@@ -1297,7 +1296,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>9821</v>
       </c>
@@ -1314,7 +1313,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>9825</v>
       </c>
@@ -1331,7 +1330,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>9844</v>
       </c>
@@ -1348,7 +1347,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>9845</v>
       </c>
@@ -1365,7 +1364,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>9846</v>
       </c>
@@ -1382,7 +1381,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>51</v>
       </c>
@@ -1399,7 +1398,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>9120</v>
       </c>
@@ -1416,7 +1415,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>9126</v>
       </c>
@@ -1433,7 +1432,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>9122</v>
       </c>
@@ -1450,7 +1449,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>9128</v>
       </c>
@@ -1467,7 +1466,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>9140</v>
       </c>
@@ -1484,7 +1483,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>9146</v>
       </c>
@@ -1501,7 +1500,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>59</v>
       </c>
@@ -1518,7 +1517,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>59</v>
       </c>
@@ -1535,7 +1534,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>9225</v>
       </c>
@@ -1552,7 +1551,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>9226</v>
       </c>
@@ -1569,7 +1568,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>9420</v>
       </c>
@@ -1586,7 +1585,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>9424</v>
       </c>
@@ -1603,7 +1602,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>9430</v>
       </c>
@@ -1620,7 +1619,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>9434</v>
       </c>
@@ -1637,7 +1636,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>9422</v>
       </c>
@@ -1654,7 +1653,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>9426</v>
       </c>
@@ -1671,7 +1670,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>9444</v>
       </c>
@@ -1688,7 +1687,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>9454</v>
       </c>
@@ -1705,7 +1704,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>9446</v>
       </c>
@@ -1722,7 +1721,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>9301</v>
       </c>
@@ -1739,7 +1738,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>9313</v>
       </c>
@@ -1756,7 +1755,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>9300</v>
       </c>
@@ -1773,7 +1772,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>9306</v>
       </c>
@@ -1790,7 +1789,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>9314</v>
       </c>
@@ -1807,7 +1806,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>9316</v>
       </c>
@@ -1824,7 +1823,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>9260</v>
       </c>
@@ -1841,7 +1840,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>9264</v>
       </c>
@@ -1858,7 +1857,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>9262</v>
       </c>
@@ -1875,7 +1874,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>9720</v>
       </c>
@@ -1892,7 +1891,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>9724</v>
       </c>
@@ -1909,7 +1908,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>9732</v>
       </c>
@@ -1926,7 +1925,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>9736</v>
       </c>
@@ -1943,7 +1942,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>9722</v>
       </c>
@@ -1960,7 +1959,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>9738</v>
       </c>
@@ -1977,7 +1976,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>9335</v>
       </c>
@@ -1994,7 +1993,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>95</v>
       </c>

</xml_diff>

<commit_message>
debugged staging smoke test
</commit_message>
<xml_diff>
--- a/Data Files/stagingMSRPs.xlsx
+++ b/Data Files/stagingMSRPs.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zsmith/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmith\Desktop\katalon_lexc\katalon_lexc_msrp\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1206DDCD-DA0E-D146-9F1D-CBF7C100383D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="13200"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="98">
   <si>
     <t>RC 300 RWD</t>
   </si>
@@ -324,7 +323,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
@@ -649,21 +648,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
     <col min="4" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>88</v>
       </c>
@@ -680,7 +679,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>9202</v>
       </c>
@@ -697,7 +696,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>9203</v>
       </c>
@@ -714,7 +713,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>9206</v>
       </c>
@@ -731,7 +730,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9207</v>
       </c>
@@ -748,7 +747,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>9212</v>
       </c>
@@ -765,7 +764,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>9213</v>
       </c>
@@ -782,7 +781,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9216</v>
       </c>
@@ -799,7 +798,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9217</v>
       </c>
@@ -816,7 +815,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9000</v>
       </c>
@@ -833,7 +832,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9002</v>
       </c>
@@ -850,7 +849,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9004</v>
       </c>
@@ -867,7 +866,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9040</v>
       </c>
@@ -884,7 +883,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>9042</v>
       </c>
@@ -901,7 +900,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>9044</v>
       </c>
@@ -918,7 +917,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>9005</v>
       </c>
@@ -935,7 +934,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>9502</v>
       </c>
@@ -952,7 +951,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -969,7 +968,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>9506</v>
       </c>
@@ -986,7 +985,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1003,7 +1002,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>9510</v>
       </c>
@@ -1020,7 +1019,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1037,7 +1036,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>9516</v>
       </c>
@@ -1054,7 +1053,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1071,7 +1070,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -1085,7 +1084,7 @@
         <v>45200</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1099,7 +1098,7 @@
         <v>47250</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1113,7 +1112,7 @@
         <v>49415</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1127,7 +1126,7 @@
         <v>50155</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>9700</v>
       </c>
@@ -1138,13 +1137,13 @@
         <v>2020</v>
       </c>
       <c r="D29" s="2">
-        <v>53000</v>
+        <v>53100</v>
       </c>
       <c r="E29" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -1155,13 +1154,13 @@
         <v>2020</v>
       </c>
       <c r="D30" s="2">
-        <v>55790</v>
+        <v>55890</v>
       </c>
       <c r="E30" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>9710</v>
       </c>
@@ -1172,13 +1171,13 @@
         <v>2020</v>
       </c>
       <c r="D31" s="2">
-        <v>64265</v>
+        <v>64365</v>
       </c>
       <c r="E31" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>9625</v>
       </c>
@@ -1189,13 +1188,13 @@
         <v>2020</v>
       </c>
       <c r="D32" s="2">
-        <v>86480</v>
+        <v>86580</v>
       </c>
       <c r="E32" s="1">
-        <v>1295</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>9620</v>
       </c>
@@ -1206,13 +1205,13 @@
         <v>2020</v>
       </c>
       <c r="D33" s="2">
-        <v>91480</v>
+        <v>91580</v>
       </c>
       <c r="E33" s="1">
-        <v>1295</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -1222,14 +1221,14 @@
       <c r="C34">
         <v>2020</v>
       </c>
-      <c r="D34" t="s">
-        <v>87</v>
+      <c r="D34" s="2">
+        <v>99310</v>
       </c>
       <c r="E34" s="1">
-        <v>1295</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>9820</v>
       </c>
@@ -1246,7 +1245,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>9824</v>
       </c>
@@ -1263,7 +1262,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>9830</v>
       </c>
@@ -1280,7 +1279,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>9834</v>
       </c>
@@ -1297,7 +1296,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>9821</v>
       </c>
@@ -1314,7 +1313,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>9825</v>
       </c>
@@ -1331,7 +1330,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>9844</v>
       </c>
@@ -1348,7 +1347,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>9845</v>
       </c>
@@ -1365,7 +1364,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>9846</v>
       </c>
@@ -1382,7 +1381,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>51</v>
       </c>
@@ -1399,7 +1398,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>9120</v>
       </c>
@@ -1416,7 +1415,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>9126</v>
       </c>
@@ -1433,7 +1432,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>9122</v>
       </c>
@@ -1450,7 +1449,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>9128</v>
       </c>
@@ -1467,7 +1466,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>9140</v>
       </c>
@@ -1484,7 +1483,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>9146</v>
       </c>
@@ -1501,7 +1500,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>59</v>
       </c>
@@ -1518,7 +1517,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>59</v>
       </c>
@@ -1535,7 +1534,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>9225</v>
       </c>
@@ -1552,7 +1551,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>9226</v>
       </c>
@@ -1569,7 +1568,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>9420</v>
       </c>
@@ -1586,7 +1585,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>9424</v>
       </c>
@@ -1603,7 +1602,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>9430</v>
       </c>
@@ -1620,7 +1619,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>9434</v>
       </c>
@@ -1637,7 +1636,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>9422</v>
       </c>
@@ -1654,7 +1653,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>9426</v>
       </c>
@@ -1671,7 +1670,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>9444</v>
       </c>
@@ -1688,7 +1687,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>9454</v>
       </c>
@@ -1705,7 +1704,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>9446</v>
       </c>
@@ -1722,7 +1721,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>9301</v>
       </c>
@@ -1739,7 +1738,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>9313</v>
       </c>
@@ -1756,7 +1755,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>9300</v>
       </c>
@@ -1773,7 +1772,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>9306</v>
       </c>
@@ -1790,7 +1789,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>9314</v>
       </c>
@@ -1807,7 +1806,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>9316</v>
       </c>
@@ -1824,7 +1823,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>9260</v>
       </c>
@@ -1841,7 +1840,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>9264</v>
       </c>
@@ -1858,7 +1857,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>9262</v>
       </c>
@@ -1875,7 +1874,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>9720</v>
       </c>
@@ -1892,7 +1891,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>9724</v>
       </c>
@@ -1909,7 +1908,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>9732</v>
       </c>
@@ -1926,7 +1925,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>9736</v>
       </c>
@@ -1943,7 +1942,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>9722</v>
       </c>
@@ -1960,7 +1959,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>9738</v>
       </c>
@@ -1977,7 +1976,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>9335</v>
       </c>
@@ -1994,7 +1993,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>95</v>
       </c>

</xml_diff>

<commit_message>
gx-lx model page, compare deactivation
</commit_message>
<xml_diff>
--- a/Data Files/stagingMSRPs.xlsx
+++ b/Data Files/stagingMSRPs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmith\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmith\Desktop\katalon_lexc\katalon_lexc_msrp\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -652,7 +652,7 @@
   <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,7 +1222,7 @@
         <v>2020</v>
       </c>
       <c r="D34" s="2">
-        <v>94475</v>
+        <v>99310</v>
       </c>
       <c r="E34" s="1">
         <v>1025</v>

</xml_diff>

<commit_message>
debugged and activated styles model tab test
</commit_message>
<xml_diff>
--- a/Data Files/stagingMSRPs.xlsx
+++ b/Data Files/stagingMSRPs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmith\Desktop\katalon_lexc\katalon_lexc_modelpage_es\Data Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmith\Desktop\katalon_lexc\katalon_lexc_msrp\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="115">
   <si>
     <t>RC 300 RWD</t>
   </si>
@@ -351,6 +351,24 @@
   </si>
   <si>
     <t>RX 450hL LUXURY AWD</t>
+  </si>
+  <si>
+    <t>RX 350 F SPORT BLACK LINE SPECIAL EDITION</t>
+  </si>
+  <si>
+    <t>RX 450h F SPORT AWD BLACK LINE SPECIAL EDITION</t>
+  </si>
+  <si>
+    <t>9422SE</t>
+  </si>
+  <si>
+    <t>9426SE</t>
+  </si>
+  <si>
+    <t>9446SE</t>
+  </si>
+  <si>
+    <t>9005SE</t>
   </si>
 </sst>
 </file>
@@ -686,14 +704,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" customWidth="1"/>
     <col min="4" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2114,6 +2132,9 @@
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>114</v>
+      </c>
       <c r="B85" t="s">
         <v>101</v>
       </c>
@@ -2121,7 +2142,7 @@
         <v>2021</v>
       </c>
       <c r="D85" s="5">
-        <v>45700</v>
+        <v>46550</v>
       </c>
       <c r="E85" s="1">
         <v>1025</v>
@@ -2231,12 +2252,57 @@
       <c r="J91" s="1"/>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>111</v>
+      </c>
+      <c r="B92" t="s">
+        <v>109</v>
+      </c>
+      <c r="C92">
+        <v>2021</v>
+      </c>
+      <c r="D92" s="5">
+        <v>49235</v>
+      </c>
+      <c r="E92" s="1">
+        <v>1025</v>
+      </c>
       <c r="K92" s="1"/>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>112</v>
+      </c>
+      <c r="B93" t="s">
+        <v>109</v>
+      </c>
+      <c r="C93">
+        <v>2021</v>
+      </c>
+      <c r="D93" s="5">
+        <v>50635</v>
+      </c>
+      <c r="E93" s="1">
+        <v>1025</v>
+      </c>
       <c r="K93" s="1"/>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>113</v>
+      </c>
+      <c r="B94" t="s">
+        <v>110</v>
+      </c>
+      <c r="C94">
+        <v>2021</v>
+      </c>
+      <c r="D94" s="5">
+        <v>51885</v>
+      </c>
+      <c r="E94" s="1">
+        <v>1025</v>
+      </c>
       <c r="K94" s="1"/>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
compare updates for es, rx, gx
</commit_message>
<xml_diff>
--- a/Data Files/stagingMSRPs.xlsx
+++ b/Data Files/stagingMSRPs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
   <si>
     <t>RC 300 RWD</t>
   </si>
@@ -369,6 +369,9 @@
   </si>
   <si>
     <t>9005SE</t>
+  </si>
+  <si>
+    <t>RX 350 AWD F SPORT BLACK LINE SPECIAL EDITION</t>
   </si>
 </sst>
 </file>
@@ -704,14 +707,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" customWidth="1"/>
+    <col min="2" max="2" width="55" customWidth="1"/>
     <col min="4" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2274,7 +2277,7 @@
         <v>112</v>
       </c>
       <c r="B93" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C93">
         <v>2021</v>

</xml_diff>

<commit_message>
prod smoke test - platform testing
</commit_message>
<xml_diff>
--- a/Data Files/stagingMSRPs.xlsx
+++ b/Data Files/stagingMSRPs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="124">
   <si>
     <t>RC 300 RWD</t>
   </si>
@@ -372,6 +372,30 @@
   </si>
   <si>
     <t>RX 350 AWD F SPORT BLACK LINE SPECIAL EDITION</t>
+  </si>
+  <si>
+    <t>9203SE</t>
+  </si>
+  <si>
+    <t>9207SE</t>
+  </si>
+  <si>
+    <t>9213SE</t>
+  </si>
+  <si>
+    <t>9217SE</t>
+  </si>
+  <si>
+    <t>RC 300 F SPORT Black Line</t>
+  </si>
+  <si>
+    <t>RC 300 AWD F SPORT Black Line</t>
+  </si>
+  <si>
+    <t>RC 350 F SPORT Black Line</t>
+  </si>
+  <si>
+    <t>RC 350 AWD F SPORT Black Line</t>
   </si>
 </sst>
 </file>
@@ -705,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K95"/>
+  <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,10 +767,10 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D2" s="2">
-        <v>41295</v>
+        <v>42120</v>
       </c>
       <c r="E2" s="1">
         <v>1025</v>
@@ -760,10 +784,10 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D3" s="2">
-        <v>46365</v>
+        <v>46590</v>
       </c>
       <c r="E3" s="1">
         <v>1025</v>
@@ -777,10 +801,10 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D4" s="2">
-        <v>43985</v>
+        <v>44810</v>
       </c>
       <c r="E4" s="1">
         <v>1025</v>
@@ -794,10 +818,10 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D5" s="2">
-        <v>48540</v>
+        <v>48765</v>
       </c>
       <c r="E5" s="1">
         <v>1025</v>
@@ -811,10 +835,10 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D6" s="2">
-        <v>44225</v>
+        <v>45050</v>
       </c>
       <c r="E6" s="1">
         <v>1025</v>
@@ -828,10 +852,10 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D7" s="2">
-        <v>49295</v>
+        <v>49520</v>
       </c>
       <c r="E7" s="1">
         <v>1025</v>
@@ -845,10 +869,10 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D8" s="2">
-        <v>46390</v>
+        <v>47215</v>
       </c>
       <c r="E8" s="1">
         <v>1025</v>
@@ -862,10 +886,10 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D9" s="2">
-        <v>50905</v>
+        <v>51130</v>
       </c>
       <c r="E9" s="1">
         <v>1025</v>
@@ -1598,10 +1622,10 @@
         <v>62</v>
       </c>
       <c r="C53">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D53" s="2">
-        <v>64900</v>
+        <v>65875</v>
       </c>
       <c r="E53" s="1">
         <v>1025</v>
@@ -1615,10 +1639,10 @@
         <v>63</v>
       </c>
       <c r="C54">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D54" s="2">
-        <v>96800</v>
+        <v>96675</v>
       </c>
       <c r="E54" s="1">
         <v>1025</v>
@@ -2309,7 +2333,73 @@
       <c r="K94" s="1"/>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>116</v>
+      </c>
+      <c r="B95" t="s">
+        <v>120</v>
+      </c>
+      <c r="C95">
+        <v>2021</v>
+      </c>
+      <c r="D95" s="5">
+        <v>48735</v>
+      </c>
+      <c r="E95" s="1">
+        <v>1025</v>
+      </c>
       <c r="K95" s="1"/>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>117</v>
+      </c>
+      <c r="B96" t="s">
+        <v>121</v>
+      </c>
+      <c r="C96">
+        <v>2021</v>
+      </c>
+      <c r="D96" s="5">
+        <v>50910</v>
+      </c>
+      <c r="E96" s="1">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>118</v>
+      </c>
+      <c r="B97" t="s">
+        <v>122</v>
+      </c>
+      <c r="C97">
+        <v>2021</v>
+      </c>
+      <c r="D97" s="5">
+        <v>51665</v>
+      </c>
+      <c r="E97" s="1">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>119</v>
+      </c>
+      <c r="B98" t="s">
+        <v>123</v>
+      </c>
+      <c r="C98">
+        <v>2021</v>
+      </c>
+      <c r="D98" s="5">
+        <v>53275</v>
+      </c>
+      <c r="E98" s="1">
+        <v>1025</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated prod smoke test browsers
</commit_message>
<xml_diff>
--- a/Data Files/stagingMSRPs.xlsx
+++ b/Data Files/stagingMSRPs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="124">
   <si>
     <t>RC 300 RWD</t>
   </si>
@@ -372,6 +372,30 @@
   </si>
   <si>
     <t>RX 350 AWD F SPORT BLACK LINE SPECIAL EDITION</t>
+  </si>
+  <si>
+    <t>9203SE</t>
+  </si>
+  <si>
+    <t>9207SE</t>
+  </si>
+  <si>
+    <t>9213SE</t>
+  </si>
+  <si>
+    <t>9217SE</t>
+  </si>
+  <si>
+    <t>RC 300 F SPORT Black Line</t>
+  </si>
+  <si>
+    <t>RC 300 AWD F SPORT Black Line</t>
+  </si>
+  <si>
+    <t>RC 350 F SPORT Black Line</t>
+  </si>
+  <si>
+    <t>RC 350 AWD F SPORT Black Line</t>
   </si>
 </sst>
 </file>
@@ -705,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K95"/>
+  <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,10 +767,10 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D2" s="2">
-        <v>41295</v>
+        <v>42120</v>
       </c>
       <c r="E2" s="1">
         <v>1025</v>
@@ -760,10 +784,10 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D3" s="2">
-        <v>46365</v>
+        <v>46590</v>
       </c>
       <c r="E3" s="1">
         <v>1025</v>
@@ -777,10 +801,10 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D4" s="2">
-        <v>43985</v>
+        <v>44810</v>
       </c>
       <c r="E4" s="1">
         <v>1025</v>
@@ -794,10 +818,10 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D5" s="2">
-        <v>48540</v>
+        <v>48765</v>
       </c>
       <c r="E5" s="1">
         <v>1025</v>
@@ -811,10 +835,10 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D6" s="2">
-        <v>44225</v>
+        <v>45050</v>
       </c>
       <c r="E6" s="1">
         <v>1025</v>
@@ -828,10 +852,10 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D7" s="2">
-        <v>49295</v>
+        <v>49520</v>
       </c>
       <c r="E7" s="1">
         <v>1025</v>
@@ -845,10 +869,10 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D8" s="2">
-        <v>46390</v>
+        <v>47215</v>
       </c>
       <c r="E8" s="1">
         <v>1025</v>
@@ -862,10 +886,10 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D9" s="2">
-        <v>50905</v>
+        <v>51130</v>
       </c>
       <c r="E9" s="1">
         <v>1025</v>
@@ -1598,10 +1622,10 @@
         <v>62</v>
       </c>
       <c r="C53">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D53" s="2">
-        <v>64900</v>
+        <v>65875</v>
       </c>
       <c r="E53" s="1">
         <v>1025</v>
@@ -1615,10 +1639,10 @@
         <v>63</v>
       </c>
       <c r="C54">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D54" s="2">
-        <v>96800</v>
+        <v>96675</v>
       </c>
       <c r="E54" s="1">
         <v>1025</v>
@@ -2309,7 +2333,73 @@
       <c r="K94" s="1"/>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>116</v>
+      </c>
+      <c r="B95" t="s">
+        <v>120</v>
+      </c>
+      <c r="C95">
+        <v>2021</v>
+      </c>
+      <c r="D95" s="5">
+        <v>48735</v>
+      </c>
+      <c r="E95" s="1">
+        <v>1025</v>
+      </c>
       <c r="K95" s="1"/>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>117</v>
+      </c>
+      <c r="B96" t="s">
+        <v>121</v>
+      </c>
+      <c r="C96">
+        <v>2021</v>
+      </c>
+      <c r="D96" s="5">
+        <v>50910</v>
+      </c>
+      <c r="E96" s="1">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>118</v>
+      </c>
+      <c r="B97" t="s">
+        <v>122</v>
+      </c>
+      <c r="C97">
+        <v>2021</v>
+      </c>
+      <c r="D97" s="5">
+        <v>51665</v>
+      </c>
+      <c r="E97" s="1">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>119</v>
+      </c>
+      <c r="B98" t="s">
+        <v>123</v>
+      </c>
+      <c r="C98">
+        <v>2021</v>
+      </c>
+      <c r="D98" s="5">
+        <v>53275</v>
+      </c>
+      <c r="E98" s="1">
+        <v>1025</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
form deeplink test added
</commit_message>
<xml_diff>
--- a/Data Files/stagingMSRPs.xlsx
+++ b/Data Files/stagingMSRPs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="124">
   <si>
     <t>RC 300 RWD</t>
   </si>
@@ -372,6 +372,30 @@
   </si>
   <si>
     <t>RX 350 AWD F SPORT BLACK LINE SPECIAL EDITION</t>
+  </si>
+  <si>
+    <t>9203SE</t>
+  </si>
+  <si>
+    <t>9207SE</t>
+  </si>
+  <si>
+    <t>9213SE</t>
+  </si>
+  <si>
+    <t>9217SE</t>
+  </si>
+  <si>
+    <t>RC 300 F SPORT Black Line</t>
+  </si>
+  <si>
+    <t>RC 300 AWD F SPORT Black Line</t>
+  </si>
+  <si>
+    <t>RC 350 F SPORT Black Line</t>
+  </si>
+  <si>
+    <t>RC 350 AWD F SPORT Black Line</t>
   </si>
 </sst>
 </file>
@@ -705,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K95"/>
+  <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,10 +767,10 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D2" s="2">
-        <v>41295</v>
+        <v>42120</v>
       </c>
       <c r="E2" s="1">
         <v>1025</v>
@@ -760,10 +784,10 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D3" s="2">
-        <v>46365</v>
+        <v>46590</v>
       </c>
       <c r="E3" s="1">
         <v>1025</v>
@@ -777,10 +801,10 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D4" s="2">
-        <v>43985</v>
+        <v>44810</v>
       </c>
       <c r="E4" s="1">
         <v>1025</v>
@@ -794,10 +818,10 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D5" s="2">
-        <v>48540</v>
+        <v>48765</v>
       </c>
       <c r="E5" s="1">
         <v>1025</v>
@@ -811,10 +835,10 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D6" s="2">
-        <v>44225</v>
+        <v>45050</v>
       </c>
       <c r="E6" s="1">
         <v>1025</v>
@@ -828,10 +852,10 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D7" s="2">
-        <v>49295</v>
+        <v>49520</v>
       </c>
       <c r="E7" s="1">
         <v>1025</v>
@@ -845,10 +869,10 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D8" s="2">
-        <v>46390</v>
+        <v>47215</v>
       </c>
       <c r="E8" s="1">
         <v>1025</v>
@@ -862,10 +886,10 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D9" s="2">
-        <v>50905</v>
+        <v>51130</v>
       </c>
       <c r="E9" s="1">
         <v>1025</v>
@@ -1598,10 +1622,10 @@
         <v>62</v>
       </c>
       <c r="C53">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D53" s="2">
-        <v>64900</v>
+        <v>65875</v>
       </c>
       <c r="E53" s="1">
         <v>1025</v>
@@ -1615,10 +1639,10 @@
         <v>63</v>
       </c>
       <c r="C54">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D54" s="2">
-        <v>96800</v>
+        <v>96675</v>
       </c>
       <c r="E54" s="1">
         <v>1025</v>
@@ -2309,7 +2333,73 @@
       <c r="K94" s="1"/>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>116</v>
+      </c>
+      <c r="B95" t="s">
+        <v>120</v>
+      </c>
+      <c r="C95">
+        <v>2021</v>
+      </c>
+      <c r="D95" s="5">
+        <v>48735</v>
+      </c>
+      <c r="E95" s="1">
+        <v>1025</v>
+      </c>
       <c r="K95" s="1"/>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>117</v>
+      </c>
+      <c r="B96" t="s">
+        <v>121</v>
+      </c>
+      <c r="C96">
+        <v>2021</v>
+      </c>
+      <c r="D96" s="5">
+        <v>50910</v>
+      </c>
+      <c r="E96" s="1">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>118</v>
+      </c>
+      <c r="B97" t="s">
+        <v>122</v>
+      </c>
+      <c r="C97">
+        <v>2021</v>
+      </c>
+      <c r="D97" s="5">
+        <v>51665</v>
+      </c>
+      <c r="E97" s="1">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>119</v>
+      </c>
+      <c r="B98" t="s">
+        <v>123</v>
+      </c>
+      <c r="C98">
+        <v>2021</v>
+      </c>
+      <c r="D98" s="5">
+        <v>53275</v>
+      </c>
+      <c r="E98" s="1">
+        <v>1025</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
form deeplink tests added
</commit_message>
<xml_diff>
--- a/Data Files/stagingMSRPs.xlsx
+++ b/Data Files/stagingMSRPs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="124">
   <si>
     <t>RC 300 RWD</t>
   </si>
@@ -372,6 +372,30 @@
   </si>
   <si>
     <t>RX 350 AWD F SPORT BLACK LINE SPECIAL EDITION</t>
+  </si>
+  <si>
+    <t>9203SE</t>
+  </si>
+  <si>
+    <t>9207SE</t>
+  </si>
+  <si>
+    <t>9213SE</t>
+  </si>
+  <si>
+    <t>9217SE</t>
+  </si>
+  <si>
+    <t>RC 300 F SPORT Black Line</t>
+  </si>
+  <si>
+    <t>RC 300 AWD F SPORT Black Line</t>
+  </si>
+  <si>
+    <t>RC 350 F SPORT Black Line</t>
+  </si>
+  <si>
+    <t>RC 350 AWD F SPORT Black Line</t>
   </si>
 </sst>
 </file>
@@ -705,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K95"/>
+  <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,10 +767,10 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D2" s="2">
-        <v>41295</v>
+        <v>42120</v>
       </c>
       <c r="E2" s="1">
         <v>1025</v>
@@ -760,10 +784,10 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D3" s="2">
-        <v>46365</v>
+        <v>46590</v>
       </c>
       <c r="E3" s="1">
         <v>1025</v>
@@ -777,10 +801,10 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D4" s="2">
-        <v>43985</v>
+        <v>44810</v>
       </c>
       <c r="E4" s="1">
         <v>1025</v>
@@ -794,10 +818,10 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D5" s="2">
-        <v>48540</v>
+        <v>48765</v>
       </c>
       <c r="E5" s="1">
         <v>1025</v>
@@ -811,10 +835,10 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D6" s="2">
-        <v>44225</v>
+        <v>45050</v>
       </c>
       <c r="E6" s="1">
         <v>1025</v>
@@ -828,10 +852,10 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D7" s="2">
-        <v>49295</v>
+        <v>49520</v>
       </c>
       <c r="E7" s="1">
         <v>1025</v>
@@ -845,10 +869,10 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D8" s="2">
-        <v>46390</v>
+        <v>47215</v>
       </c>
       <c r="E8" s="1">
         <v>1025</v>
@@ -862,10 +886,10 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D9" s="2">
-        <v>50905</v>
+        <v>51130</v>
       </c>
       <c r="E9" s="1">
         <v>1025</v>
@@ -1598,10 +1622,10 @@
         <v>62</v>
       </c>
       <c r="C53">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D53" s="2">
-        <v>64900</v>
+        <v>65875</v>
       </c>
       <c r="E53" s="1">
         <v>1025</v>
@@ -1615,10 +1639,10 @@
         <v>63</v>
       </c>
       <c r="C54">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D54" s="2">
-        <v>96800</v>
+        <v>96675</v>
       </c>
       <c r="E54" s="1">
         <v>1025</v>
@@ -2309,7 +2333,73 @@
       <c r="K94" s="1"/>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>116</v>
+      </c>
+      <c r="B95" t="s">
+        <v>120</v>
+      </c>
+      <c r="C95">
+        <v>2021</v>
+      </c>
+      <c r="D95" s="5">
+        <v>48735</v>
+      </c>
+      <c r="E95" s="1">
+        <v>1025</v>
+      </c>
       <c r="K95" s="1"/>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>117</v>
+      </c>
+      <c r="B96" t="s">
+        <v>121</v>
+      </c>
+      <c r="C96">
+        <v>2021</v>
+      </c>
+      <c r="D96" s="5">
+        <v>50910</v>
+      </c>
+      <c r="E96" s="1">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>118</v>
+      </c>
+      <c r="B97" t="s">
+        <v>122</v>
+      </c>
+      <c r="C97">
+        <v>2021</v>
+      </c>
+      <c r="D97" s="5">
+        <v>51665</v>
+      </c>
+      <c r="E97" s="1">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>119</v>
+      </c>
+      <c r="B98" t="s">
+        <v>123</v>
+      </c>
+      <c r="C98">
+        <v>2021</v>
+      </c>
+      <c r="D98" s="5">
+        <v>53275</v>
+      </c>
+      <c r="E98" s="1">
+        <v>1025</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
vehicle shown pricing adjustments
</commit_message>
<xml_diff>
--- a/Data Files/stagingMSRPs.xlsx
+++ b/Data Files/stagingMSRPs.xlsx
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1642,7 +1642,7 @@
         <v>2021</v>
       </c>
       <c r="D54" s="2">
-        <v>96675</v>
+        <v>97100</v>
       </c>
       <c r="E54" s="1">
         <v>1025</v>

</xml_diff>

<commit_message>
updated black line pricing data
</commit_message>
<xml_diff>
--- a/Data Files/stagingMSRPs.xlsx
+++ b/Data Files/stagingMSRPs.xlsx
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2343,7 +2343,7 @@
         <v>2021</v>
       </c>
       <c r="D95" s="5">
-        <v>48735</v>
+        <v>49160</v>
       </c>
       <c r="E95" s="1">
         <v>1025</v>
@@ -2361,7 +2361,7 @@
         <v>2021</v>
       </c>
       <c r="D96" s="5">
-        <v>50910</v>
+        <v>51335</v>
       </c>
       <c r="E96" s="1">
         <v>1025</v>
@@ -2378,7 +2378,7 @@
         <v>2021</v>
       </c>
       <c r="D97" s="5">
-        <v>51665</v>
+        <v>52090</v>
       </c>
       <c r="E97" s="1">
         <v>1025</v>
@@ -2395,7 +2395,7 @@
         <v>2021</v>
       </c>
       <c r="D98" s="5">
-        <v>53275</v>
+        <v>53700</v>
       </c>
       <c r="E98" s="1">
         <v>1025</v>

</xml_diff>

<commit_message>
staging smoke test setup
</commit_message>
<xml_diff>
--- a/Data Files/stagingMSRPs.xlsx
+++ b/Data Files/stagingMSRPs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="122">
   <si>
     <t>RC 300 RWD</t>
   </si>
@@ -71,9 +71,6 @@
     <t>ES 350 F SPORT</t>
   </si>
   <si>
-    <t>IS 300</t>
-  </si>
-  <si>
     <t>9502FK or v9502F</t>
   </si>
   <si>
@@ -89,18 +86,12 @@
     <t>IS 300 F SPORT AWD</t>
   </si>
   <si>
-    <t>IS 350 RWD</t>
-  </si>
-  <si>
     <t>9510FK or v9510F</t>
   </si>
   <si>
     <t>IS 350 F SPORT RWD</t>
   </si>
   <si>
-    <t>IS 350 AWD</t>
-  </si>
-  <si>
     <t>9516FJ or v9516F</t>
   </si>
   <si>
@@ -396,6 +387,9 @@
   </si>
   <si>
     <t>RC F FUJI SPEEDWAY EDITION</t>
+  </si>
+  <si>
+    <t>IS 300 RWD</t>
   </si>
 </sst>
 </file>
@@ -731,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D99" sqref="D99"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,19 +738,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" t="s">
         <v>87</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>88</v>
-      </c>
-      <c r="C1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1019,13 +1013,13 @@
         <v>9502</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>121</v>
       </c>
       <c r="C17">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D17" s="2">
-        <v>38560</v>
+        <v>39000</v>
       </c>
       <c r="E17" s="1">
         <v>1025</v>
@@ -1033,10 +1027,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
         <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>17</v>
       </c>
       <c r="C18">
         <v>2020</v>
@@ -1053,13 +1047,13 @@
         <v>9506</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D19" s="2">
-        <v>41010</v>
+        <v>41000</v>
       </c>
       <c r="E19" s="1">
         <v>1025</v>
@@ -1067,10 +1061,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
         <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>20</v>
       </c>
       <c r="C20">
         <v>2020</v>
@@ -1090,10 +1084,10 @@
         <v>21</v>
       </c>
       <c r="C21">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D21" s="2">
-        <v>42180</v>
+        <v>42900</v>
       </c>
       <c r="E21" s="1">
         <v>1025</v>
@@ -1101,10 +1095,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C22">
         <v>2020</v>
@@ -1121,13 +1115,13 @@
         <v>9516</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D23" s="2">
-        <v>44345</v>
+        <v>44900</v>
       </c>
       <c r="E23" s="1">
         <v>1025</v>
@@ -1135,10 +1129,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C24">
         <v>2020</v>
@@ -1152,10 +1146,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C25">
         <v>2020</v>
@@ -1166,10 +1160,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C26">
         <v>2020</v>
@@ -1180,10 +1174,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C27">
         <v>2020</v>
@@ -1194,10 +1188,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C28">
         <v>2020</v>
@@ -1211,7 +1205,7 @@
         <v>9700</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C29">
         <v>2020</v>
@@ -1225,10 +1219,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C30">
         <v>2020</v>
@@ -1245,7 +1239,7 @@
         <v>9710</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C31">
         <v>2020</v>
@@ -1262,7 +1256,7 @@
         <v>9625</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C32">
         <v>2020</v>
@@ -1279,7 +1273,7 @@
         <v>9620</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C33">
         <v>2020</v>
@@ -1293,10 +1287,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C34">
         <v>2020</v>
@@ -1313,7 +1307,7 @@
         <v>9820</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C35">
         <v>2021</v>
@@ -1330,7 +1324,7 @@
         <v>9824</v>
       </c>
       <c r="B36" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C36">
         <v>2021</v>
@@ -1347,7 +1341,7 @@
         <v>9830</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C37">
         <v>2021</v>
@@ -1364,7 +1358,7 @@
         <v>9834</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C38">
         <v>2021</v>
@@ -1381,7 +1375,7 @@
         <v>9821</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C39">
         <v>2021</v>
@@ -1398,7 +1392,7 @@
         <v>9825</v>
       </c>
       <c r="B40" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C40">
         <v>2021</v>
@@ -1415,7 +1409,7 @@
         <v>9844</v>
       </c>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C41">
         <v>2021</v>
@@ -1432,7 +1426,7 @@
         <v>9845</v>
       </c>
       <c r="B42" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C42">
         <v>2021</v>
@@ -1449,7 +1443,7 @@
         <v>9846</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C43">
         <v>2021</v>
@@ -1463,10 +1457,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B44" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C44">
         <v>2020</v>
@@ -1483,7 +1477,7 @@
         <v>9120</v>
       </c>
       <c r="B45" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C45">
         <v>2020</v>
@@ -1500,7 +1494,7 @@
         <v>9126</v>
       </c>
       <c r="B46" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C46">
         <v>2020</v>
@@ -1517,7 +1511,7 @@
         <v>9122</v>
       </c>
       <c r="B47" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C47">
         <v>2020</v>
@@ -1534,7 +1528,7 @@
         <v>9128</v>
       </c>
       <c r="B48" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C48">
         <v>2020</v>
@@ -1551,7 +1545,7 @@
         <v>9140</v>
       </c>
       <c r="B49" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C49">
         <v>2020</v>
@@ -1568,7 +1562,7 @@
         <v>9146</v>
       </c>
       <c r="B50" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C50">
         <v>2020</v>
@@ -1582,10 +1576,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B51" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C51">
         <v>2020</v>
@@ -1599,10 +1593,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B52" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C52">
         <v>2020</v>
@@ -1619,7 +1613,7 @@
         <v>9225</v>
       </c>
       <c r="B53" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C53">
         <v>2021</v>
@@ -1636,7 +1630,7 @@
         <v>9226</v>
       </c>
       <c r="B54" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C54">
         <v>2021</v>
@@ -1653,7 +1647,7 @@
         <v>9420</v>
       </c>
       <c r="B55" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C55">
         <v>2021</v>
@@ -1670,7 +1664,7 @@
         <v>9424</v>
       </c>
       <c r="B56" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C56">
         <v>2021</v>
@@ -1687,7 +1681,7 @@
         <v>9430</v>
       </c>
       <c r="B57" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C57">
         <v>2021</v>
@@ -1704,7 +1698,7 @@
         <v>9434</v>
       </c>
       <c r="B58" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C58">
         <v>2021</v>
@@ -1721,7 +1715,7 @@
         <v>9422</v>
       </c>
       <c r="B59" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C59">
         <v>2021</v>
@@ -1738,7 +1732,7 @@
         <v>9426</v>
       </c>
       <c r="B60" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C60">
         <v>2021</v>
@@ -1755,7 +1749,7 @@
         <v>9444</v>
       </c>
       <c r="B61" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C61">
         <v>2021</v>
@@ -1772,7 +1766,7 @@
         <v>9454</v>
       </c>
       <c r="B62" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C62">
         <v>2021</v>
@@ -1789,7 +1783,7 @@
         <v>9446</v>
       </c>
       <c r="B63" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C63">
         <v>2021</v>
@@ -1806,13 +1800,13 @@
         <v>9301</v>
       </c>
       <c r="B64" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C64">
         <v>2020</v>
       </c>
       <c r="D64" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E64" s="1">
         <v>1025</v>
@@ -1823,13 +1817,13 @@
         <v>9313</v>
       </c>
       <c r="B65" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C65">
         <v>2020</v>
       </c>
       <c r="D65" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E65" s="1">
         <v>1025</v>
@@ -1840,7 +1834,7 @@
         <v>9300</v>
       </c>
       <c r="B66" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C66">
         <v>2020</v>
@@ -1857,7 +1851,7 @@
         <v>9306</v>
       </c>
       <c r="B67" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C67">
         <v>2020</v>
@@ -1874,7 +1868,7 @@
         <v>9314</v>
       </c>
       <c r="B68" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C68">
         <v>2020</v>
@@ -1891,7 +1885,7 @@
         <v>9316</v>
       </c>
       <c r="B69" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C69">
         <v>2020</v>
@@ -1908,7 +1902,7 @@
         <v>9260</v>
       </c>
       <c r="B70" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C70">
         <v>2021</v>
@@ -1925,7 +1919,7 @@
         <v>9264</v>
       </c>
       <c r="B71" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C71">
         <v>2021</v>
@@ -1942,7 +1936,7 @@
         <v>9262</v>
       </c>
       <c r="B72" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C72">
         <v>2021</v>
@@ -1959,13 +1953,13 @@
         <v>9720</v>
       </c>
       <c r="B73" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C73">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D73" s="3">
-        <v>32300</v>
+        <v>32900</v>
       </c>
       <c r="E73" s="1">
         <v>1025</v>
@@ -1976,13 +1970,13 @@
         <v>9724</v>
       </c>
       <c r="B74" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C74">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D74" s="3">
-        <v>37500</v>
+        <v>37600</v>
       </c>
       <c r="E74" s="1">
         <v>1025</v>
@@ -1993,13 +1987,13 @@
         <v>9732</v>
       </c>
       <c r="B75" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C75">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D75" s="3">
-        <v>34500</v>
+        <v>35100</v>
       </c>
       <c r="E75" s="1">
         <v>1025</v>
@@ -2010,13 +2004,13 @@
         <v>9736</v>
       </c>
       <c r="B76" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C76">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D76" s="3">
-        <v>39700</v>
+        <v>39800</v>
       </c>
       <c r="E76" s="1">
         <v>1025</v>
@@ -2027,13 +2021,13 @@
         <v>9722</v>
       </c>
       <c r="B77" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C77">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D77" s="3">
-        <v>34300</v>
+        <v>34900</v>
       </c>
       <c r="E77" s="1">
         <v>1025</v>
@@ -2044,13 +2038,13 @@
         <v>9738</v>
       </c>
       <c r="B78" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C78">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D78" s="3">
-        <v>36500</v>
+        <v>37100</v>
       </c>
       <c r="E78" s="1">
         <v>1025</v>
@@ -2061,7 +2055,7 @@
         <v>9335</v>
       </c>
       <c r="B79" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C79">
         <v>2020</v>
@@ -2075,10 +2069,10 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B80" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C80">
         <v>2021</v>
@@ -2095,7 +2089,7 @@
         <v>9012</v>
       </c>
       <c r="B81" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C81">
         <v>2021</v>
@@ -2112,7 +2106,7 @@
         <v>9013</v>
       </c>
       <c r="B82" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C82">
         <v>2021</v>
@@ -2129,7 +2123,7 @@
         <v>9014</v>
       </c>
       <c r="B83" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C83">
         <v>2021</v>
@@ -2146,7 +2140,7 @@
         <v>9015</v>
       </c>
       <c r="B84" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C84">
         <v>2021</v>
@@ -2160,10 +2154,10 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B85" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C85">
         <v>2021</v>
@@ -2180,7 +2174,7 @@
         <v>9423</v>
       </c>
       <c r="B86" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C86">
         <v>2021</v>
@@ -2197,7 +2191,7 @@
         <v>9427</v>
       </c>
       <c r="B87" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C87">
         <v>2021</v>
@@ -2214,7 +2208,7 @@
         <v>9447</v>
       </c>
       <c r="B88" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C88">
         <v>2021</v>
@@ -2231,7 +2225,7 @@
         <v>9432</v>
       </c>
       <c r="B89" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C89">
         <v>2021</v>
@@ -2248,7 +2242,7 @@
         <v>9436</v>
       </c>
       <c r="B90" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C90">
         <v>2021</v>
@@ -2265,7 +2259,7 @@
         <v>9457</v>
       </c>
       <c r="B91" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C91">
         <v>2021</v>
@@ -2280,10 +2274,10 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B92" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C92">
         <v>2021</v>
@@ -2298,10 +2292,10 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>108</v>
+      </c>
+      <c r="B93" t="s">
         <v>111</v>
-      </c>
-      <c r="B93" t="s">
-        <v>114</v>
       </c>
       <c r="C93">
         <v>2021</v>
@@ -2316,10 +2310,10 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B94" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C94">
         <v>2021</v>
@@ -2334,10 +2328,10 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B95" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C95">
         <v>2021</v>
@@ -2352,10 +2346,10 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B96" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C96">
         <v>2021</v>
@@ -2369,10 +2363,10 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B97" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C97">
         <v>2021</v>
@@ -2386,10 +2380,10 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B98" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C98">
         <v>2021</v>

</xml_diff>

<commit_message>
deeplink and msrp tests added
</commit_message>
<xml_diff>
--- a/Data Files/stagingMSRPs.xlsx
+++ b/Data Files/stagingMSRPs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="124">
   <si>
     <t>RC 300 RWD</t>
   </si>
@@ -390,6 +390,12 @@
   </si>
   <si>
     <t>IS 300 RWD</t>
+  </si>
+  <si>
+    <t>UX 250h AWD BLACK LINE SPECIAL EDITION</t>
+  </si>
+  <si>
+    <t>COMING SOON</t>
   </si>
 </sst>
 </file>
@@ -723,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K98"/>
+  <dimension ref="A1:K99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1208,7 +1214,7 @@
         <v>32</v>
       </c>
       <c r="C29">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D29" s="2">
         <v>53100</v>
@@ -1225,10 +1231,10 @@
         <v>34</v>
       </c>
       <c r="C30">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D30" s="2">
-        <v>55890</v>
+        <v>56190</v>
       </c>
       <c r="E30" s="1">
         <v>1025</v>
@@ -1242,7 +1248,7 @@
         <v>35</v>
       </c>
       <c r="C31">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D31" s="2">
         <v>64365</v>
@@ -1480,10 +1486,10 @@
         <v>50</v>
       </c>
       <c r="C45">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D45" s="2">
-        <v>75450</v>
+        <v>76000</v>
       </c>
       <c r="E45" s="1">
         <v>1025</v>
@@ -1497,10 +1503,10 @@
         <v>51</v>
       </c>
       <c r="C46">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D46" s="2">
-        <v>78670</v>
+        <v>79250</v>
       </c>
       <c r="E46" s="1">
         <v>1025</v>
@@ -1514,10 +1520,10 @@
         <v>52</v>
       </c>
       <c r="C47">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D47" s="2">
-        <v>81450</v>
+        <v>79600</v>
       </c>
       <c r="E47" s="1">
         <v>1025</v>
@@ -1531,10 +1537,10 @@
         <v>53</v>
       </c>
       <c r="C48">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D48" s="2">
-        <v>84670</v>
+        <v>82850</v>
       </c>
       <c r="E48" s="1">
         <v>1025</v>
@@ -2392,6 +2398,20 @@
         <v>53700</v>
       </c>
       <c r="E98" s="1">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>122</v>
+      </c>
+      <c r="C99">
+        <v>2021</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E99" s="1">
         <v>1025</v>
       </c>
     </row>

</xml_diff>

<commit_message>
disabled staging compare report tests
</commit_message>
<xml_diff>
--- a/Data Files/stagingMSRPs.xlsx
+++ b/Data Files/stagingMSRPs.xlsx
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1642,7 +1642,7 @@
         <v>2021</v>
       </c>
       <c r="D54" s="2">
-        <v>97200</v>
+        <v>97625</v>
       </c>
       <c r="E54" s="1">
         <v>1025</v>
@@ -2289,7 +2289,7 @@
         <v>2021</v>
       </c>
       <c r="D92" s="5">
-        <v>49235</v>
+        <v>49335</v>
       </c>
       <c r="E92" s="1">
         <v>1025</v>
@@ -2307,7 +2307,7 @@
         <v>2021</v>
       </c>
       <c r="D93" s="5">
-        <v>50635</v>
+        <v>50735</v>
       </c>
       <c r="E93" s="1">
         <v>1025</v>
@@ -2325,7 +2325,7 @@
         <v>2021</v>
       </c>
       <c r="D94" s="5">
-        <v>51885</v>
+        <v>51985</v>
       </c>
       <c r="E94" s="1">
         <v>1025</v>

</xml_diff>

<commit_message>
set up hybrid tests
</commit_message>
<xml_diff>
--- a/Data Files/stagingMSRPs.xlsx
+++ b/Data Files/stagingMSRPs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="126">
   <si>
     <t>RC 300 RWD</t>
   </si>
@@ -396,6 +396,12 @@
   </si>
   <si>
     <t>COMING SOON</t>
+  </si>
+  <si>
+    <t>LC 500 INSPIRATION SERIES</t>
+  </si>
+  <si>
+    <t>9260LE</t>
   </si>
 </sst>
 </file>
@@ -729,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K99"/>
+  <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1554,10 +1560,10 @@
         <v>54</v>
       </c>
       <c r="C49">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D49" s="2">
-        <v>80010</v>
+        <v>90500</v>
       </c>
       <c r="E49" s="1">
         <v>1025</v>
@@ -1571,10 +1577,10 @@
         <v>55</v>
       </c>
       <c r="C50">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D50" s="2">
-        <v>83230</v>
+        <v>93750</v>
       </c>
       <c r="E50" s="1">
         <v>1025</v>
@@ -1642,7 +1648,7 @@
         <v>2021</v>
       </c>
       <c r="D54" s="2">
-        <v>97200</v>
+        <v>97625</v>
       </c>
       <c r="E54" s="1">
         <v>1025</v>
@@ -2084,7 +2090,7 @@
         <v>2021</v>
       </c>
       <c r="D80" s="2">
-        <v>119800</v>
+        <v>119900</v>
       </c>
       <c r="E80" s="1">
         <v>1025</v>
@@ -2289,7 +2295,7 @@
         <v>2021</v>
       </c>
       <c r="D92" s="5">
-        <v>49235</v>
+        <v>49335</v>
       </c>
       <c r="E92" s="1">
         <v>1025</v>
@@ -2307,7 +2313,7 @@
         <v>2021</v>
       </c>
       <c r="D93" s="5">
-        <v>50635</v>
+        <v>50735</v>
       </c>
       <c r="E93" s="1">
         <v>1025</v>
@@ -2325,7 +2331,7 @@
         <v>2021</v>
       </c>
       <c r="D94" s="5">
-        <v>51885</v>
+        <v>51985</v>
       </c>
       <c r="E94" s="1">
         <v>1025</v>
@@ -2343,7 +2349,7 @@
         <v>2021</v>
       </c>
       <c r="D95" s="5">
-        <v>49160</v>
+        <v>48835</v>
       </c>
       <c r="E95" s="1">
         <v>1025</v>
@@ -2361,7 +2367,7 @@
         <v>2021</v>
       </c>
       <c r="D96" s="5">
-        <v>51335</v>
+        <v>51010</v>
       </c>
       <c r="E96" s="1">
         <v>1025</v>
@@ -2378,7 +2384,7 @@
         <v>2021</v>
       </c>
       <c r="D97" s="5">
-        <v>52090</v>
+        <v>51765</v>
       </c>
       <c r="E97" s="1">
         <v>1025</v>
@@ -2395,7 +2401,7 @@
         <v>2021</v>
       </c>
       <c r="D98" s="5">
-        <v>53700</v>
+        <v>53230</v>
       </c>
       <c r="E98" s="1">
         <v>1025</v>
@@ -2412,6 +2418,23 @@
         <v>123</v>
       </c>
       <c r="E99" s="1">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A100" t="s">
+        <v>125</v>
+      </c>
+      <c r="B100" t="s">
+        <v>124</v>
+      </c>
+      <c r="C100">
+        <v>2021</v>
+      </c>
+      <c r="D100" s="2">
+        <v>110420</v>
+      </c>
+      <c r="E100" s="1">
         <v>1025</v>
       </c>
     </row>

</xml_diff>